<commit_message>
add broswer & license icons
</commit_message>
<xml_diff>
--- a/scripts/source.xlsx
+++ b/scripts/source.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\tomchen\GETICON\geticon\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7F7E2F-0E93-4812-BAA2-352EB4C7C795}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C27591-6668-436B-A06A-EF1F2FFDD07E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adobe" sheetId="1" r:id="rId1"/>
+    <sheet name="browsersetc" sheetId="2" r:id="rId2"/>
+    <sheet name="licenses" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="370">
   <si>
     <t>adobe-acrobat.svg</t>
   </si>
@@ -496,6 +498,645 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>alibaba.svg</t>
+  </si>
+  <si>
+    <t>baidu-logo.svg</t>
+  </si>
+  <si>
+    <t>baidu.svg</t>
+  </si>
+  <si>
+    <t>bytedance-logo.svg</t>
+  </si>
+  <si>
+    <t>bytedance.svg</t>
+  </si>
+  <si>
+    <t>chromium.svg</t>
+  </si>
+  <si>
+    <t>gecko.svg</t>
+  </si>
+  <si>
+    <t>maxthon.svg</t>
+  </si>
+  <si>
+    <t>mediawiki.svg</t>
+  </si>
+  <si>
+    <t>qq.svg</t>
+  </si>
+  <si>
+    <t>qwant-logo.svg</t>
+  </si>
+  <si>
+    <t>qwant.svg</t>
+  </si>
+  <si>
+    <t>samsung_internet.svg</t>
+  </si>
+  <si>
+    <t>sina_weibo.svg</t>
+  </si>
+  <si>
+    <t>tencent.svg</t>
+  </si>
+  <si>
+    <t>tiktok-logo.svg</t>
+  </si>
+  <si>
+    <t>tiktok.svg</t>
+  </si>
+  <si>
+    <t>tor_browser.svg</t>
+  </si>
+  <si>
+    <t>ucbrowser.svg</t>
+  </si>
+  <si>
+    <t>webgl.svg</t>
+  </si>
+  <si>
+    <t>webkit.svg</t>
+  </si>
+  <si>
+    <t>wechat-logo.svg</t>
+  </si>
+  <si>
+    <t>wechat.svg</t>
+  </si>
+  <si>
+    <t>wikimedia.svg</t>
+  </si>
+  <si>
+    <t>wikimedia_commons.svg</t>
+  </si>
+  <si>
+    <t>wikipedia.svg</t>
+  </si>
+  <si>
+    <t>yandex-logo.svg</t>
+  </si>
+  <si>
+    <t>yandex_browser.svg</t>
+  </si>
+  <si>
+    <t>agpl_v3.svg</t>
+  </si>
+  <si>
+    <t>bsd.svg</t>
+  </si>
+  <si>
+    <t>cc-0-button.svg</t>
+  </si>
+  <si>
+    <t>cc-0-icon.svg</t>
+  </si>
+  <si>
+    <t>cc-by-button.svg</t>
+  </si>
+  <si>
+    <t>cc-by-icon.svg</t>
+  </si>
+  <si>
+    <t>cc-by-nc-button.svg</t>
+  </si>
+  <si>
+    <t>cc-by-nc-nd-button.svg</t>
+  </si>
+  <si>
+    <t>cc-by-nc-sa-button.svg</t>
+  </si>
+  <si>
+    <t>cc-by-nd-button.svg</t>
+  </si>
+  <si>
+    <t>cc-by-sa-button.svg</t>
+  </si>
+  <si>
+    <t>cc-nc-icon.svg</t>
+  </si>
+  <si>
+    <t>cc-nd-icon.svg</t>
+  </si>
+  <si>
+    <t>cc-pd-button.svg</t>
+  </si>
+  <si>
+    <t>cc-pd-icon.svg</t>
+  </si>
+  <si>
+    <t>cc-sa-icon.svg</t>
+  </si>
+  <si>
+    <t>gfdl.svg</t>
+  </si>
+  <si>
+    <t>gpl_v3.svg</t>
+  </si>
+  <si>
+    <t>lgpl_v3.svg</t>
+  </si>
+  <si>
+    <t>mit.svg</t>
+  </si>
+  <si>
+    <t>pd-icon.svg</t>
+  </si>
+  <si>
+    <t>aliases 2</t>
+  </si>
+  <si>
+    <t>aliases 3</t>
+  </si>
+  <si>
+    <t>aliases 4</t>
+  </si>
+  <si>
+    <t>files 2</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Alibaba</t>
+  </si>
+  <si>
+    <t>alibaba</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/</t>
+  </si>
+  <si>
+    <t>baidu</t>
+  </si>
+  <si>
+    <t>bytedance</t>
+  </si>
+  <si>
+    <t>chromium</t>
+  </si>
+  <si>
+    <t>gecko</t>
+  </si>
+  <si>
+    <t>maxthon</t>
+  </si>
+  <si>
+    <t>mediawiki</t>
+  </si>
+  <si>
+    <t>qq</t>
+  </si>
+  <si>
+    <t>qwant</t>
+  </si>
+  <si>
+    <t>samsung_internet</t>
+  </si>
+  <si>
+    <t>sina_weibo</t>
+  </si>
+  <si>
+    <t>tencent</t>
+  </si>
+  <si>
+    <t>tiktok</t>
+  </si>
+  <si>
+    <t>tor_browser</t>
+  </si>
+  <si>
+    <t>ucbrowser</t>
+  </si>
+  <si>
+    <t>webgl</t>
+  </si>
+  <si>
+    <t>webkit</t>
+  </si>
+  <si>
+    <t>wechat</t>
+  </si>
+  <si>
+    <t>wikimedia</t>
+  </si>
+  <si>
+    <t>wikimedia_commons</t>
+  </si>
+  <si>
+    <t>wikipedia</t>
+  </si>
+  <si>
+    <t>yandex</t>
+  </si>
+  <si>
+    <t>yandex_browser</t>
+  </si>
+  <si>
+    <t>Baidu</t>
+  </si>
+  <si>
+    <t>Chromium</t>
+  </si>
+  <si>
+    <t>Gecko</t>
+  </si>
+  <si>
+    <t>Maxthon</t>
+  </si>
+  <si>
+    <t>MediaWiki</t>
+  </si>
+  <si>
+    <t>QQ</t>
+  </si>
+  <si>
+    <t>Qwant</t>
+  </si>
+  <si>
+    <t>Samsung Internet</t>
+  </si>
+  <si>
+    <t>Sina Weibo</t>
+  </si>
+  <si>
+    <t>Tencent</t>
+  </si>
+  <si>
+    <t>TikTok</t>
+  </si>
+  <si>
+    <t>Tor Browser</t>
+  </si>
+  <si>
+    <t>UC Browser</t>
+  </si>
+  <si>
+    <t>WebGL</t>
+  </si>
+  <si>
+    <t>WebKit</t>
+  </si>
+  <si>
+    <t>WeChat</t>
+  </si>
+  <si>
+    <t>Wikimedia</t>
+  </si>
+  <si>
+    <t>Wikimedia Commons</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Yandex</t>
+  </si>
+  <si>
+    <t>Yandex Browser</t>
+  </si>
+  <si>
+    <t>https://www.baidu.com/</t>
+  </si>
+  <si>
+    <t>ByteDance</t>
+  </si>
+  <si>
+    <t>https://www.bytedance.com/</t>
+  </si>
+  <si>
+    <t>https://www.chromium.org/</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Mozilla/Gecko</t>
+  </si>
+  <si>
+    <t>https://www.maxthon.com/</t>
+  </si>
+  <si>
+    <t>https://www.mediawiki.org/wiki/MediaWiki</t>
+  </si>
+  <si>
+    <t>https://im.qq.com/</t>
+  </si>
+  <si>
+    <t>https://www.qwant.com/</t>
+  </si>
+  <si>
+    <t>https://www.samsung.com/us/support/owners/app/samsung-internet</t>
+  </si>
+  <si>
+    <t>https://weibo.com/</t>
+  </si>
+  <si>
+    <t>https://www.tencent.com/</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/</t>
+  </si>
+  <si>
+    <t>https://www.torproject.org/</t>
+  </si>
+  <si>
+    <t>http://www.ucweb.com/</t>
+  </si>
+  <si>
+    <t>https://www.khronos.org/webgl/</t>
+  </si>
+  <si>
+    <t>https://webkit.org/</t>
+  </si>
+  <si>
+    <t>https://www.wechat.com/</t>
+  </si>
+  <si>
+    <t>https://www.wikimedia.org/</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/</t>
+  </si>
+  <si>
+    <t>https://www.wikipedia.org/</t>
+  </si>
+  <si>
+    <t>https://yandex.com/</t>
+  </si>
+  <si>
+    <t>https://browser.yandex.com/</t>
+  </si>
+  <si>
+    <t>阿里巴巴</t>
+  </si>
+  <si>
+    <t>阿里</t>
+  </si>
+  <si>
+    <t>百度</t>
+  </si>
+  <si>
+    <t>字节跳动</t>
+  </si>
+  <si>
+    <t>傲游</t>
+  </si>
+  <si>
+    <t>傲游浏览器</t>
+  </si>
+  <si>
+    <t>MyIE2</t>
+  </si>
+  <si>
+    <t>Weibo</t>
+  </si>
+  <si>
+    <t>微博</t>
+  </si>
+  <si>
+    <t>新浪微博</t>
+  </si>
+  <si>
+    <t>腾讯</t>
+  </si>
+  <si>
+    <t>抖音</t>
+  </si>
+  <si>
+    <t>UC浏览器</t>
+  </si>
+  <si>
+    <t>微信</t>
+  </si>
+  <si>
+    <t>agpl_v3</t>
+  </si>
+  <si>
+    <t>bsd</t>
+  </si>
+  <si>
+    <t>cc-0</t>
+  </si>
+  <si>
+    <t>cc-0-icon</t>
+  </si>
+  <si>
+    <t>cc-by</t>
+  </si>
+  <si>
+    <t>cc-by-icon</t>
+  </si>
+  <si>
+    <t>cc-by-nc</t>
+  </si>
+  <si>
+    <t>cc-by-nc-nd</t>
+  </si>
+  <si>
+    <t>cc-by-nc-sa</t>
+  </si>
+  <si>
+    <t>cc-by-nd</t>
+  </si>
+  <si>
+    <t>cc-by-sa</t>
+  </si>
+  <si>
+    <t>cc-nc-icon</t>
+  </si>
+  <si>
+    <t>cc-nd-icon</t>
+  </si>
+  <si>
+    <t>cc-pd</t>
+  </si>
+  <si>
+    <t>cc-pd-icon</t>
+  </si>
+  <si>
+    <t>cc-sa-icon</t>
+  </si>
+  <si>
+    <t>gfdl</t>
+  </si>
+  <si>
+    <t>gpl_v3</t>
+  </si>
+  <si>
+    <t>lgpl_v3</t>
+  </si>
+  <si>
+    <t>mit</t>
+  </si>
+  <si>
+    <t>pd</t>
+  </si>
+  <si>
+    <t>AGPL v3</t>
+  </si>
+  <si>
+    <t>BSD License</t>
+  </si>
+  <si>
+    <t>GFDL</t>
+  </si>
+  <si>
+    <t>GPL v3</t>
+  </si>
+  <si>
+    <t>LGPL v3</t>
+  </si>
+  <si>
+    <t>MIT License</t>
+  </si>
+  <si>
+    <t>Public domain</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Public_domain</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/MIT</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/licenses/lgpl-3.0.html</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/licenses/gpl-3.0.html</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/licenses/fdl-1.3.html</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/licenses/agpl-3.0.html</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/BSD_licenses</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/share-your-work/public-domain/cc0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc/4.0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/publicdomain/mark/1.0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-nd/4.0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nd/4.0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-sa/4.0/</t>
+  </si>
+  <si>
+    <t>CC0</t>
+  </si>
+  <si>
+    <t>Attribution (BY)</t>
+  </si>
+  <si>
+    <t>Public domain (CC0)</t>
+  </si>
+  <si>
+    <t>Share-alike (SA)</t>
+  </si>
+  <si>
+    <t>Non-commercial (NC)</t>
+  </si>
+  <si>
+    <t>No Derivative Works (ND)</t>
+  </si>
+  <si>
+    <t>Creative Commons - Public Domain Mark</t>
+  </si>
+  <si>
+    <t>Public domain (CC)</t>
+  </si>
+  <si>
+    <t>Creative Commons - Attribution (CC-BY)</t>
+  </si>
+  <si>
+    <t>Creative Commons - Attribution-Noncommercial (CC-BY-NC)</t>
+  </si>
+  <si>
+    <t>Creative Commons - Attribution-Noncommercial-NoDerivatives (CC-BY-NC-ND)</t>
+  </si>
+  <si>
+    <t>Creative Commons - Attribution-Noncommercial-ShareAlike (CC-BY-NC-SA)</t>
+  </si>
+  <si>
+    <t>Creative Commons - Attribution-NoDerivatives (CC-BY-ND)</t>
+  </si>
+  <si>
+    <t>Creative Commons - Attribution-ShareAlike (CC-BY-SA)</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>corporation</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>search engine</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>browser engine</t>
+  </si>
+  <si>
+    <t>instant messenger</t>
+  </si>
+  <si>
+    <t>wiki</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>social media</t>
+  </si>
+  <si>
+    <t>china</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>russia</t>
+  </si>
+  <si>
+    <t>tag 1</t>
+  </si>
+  <si>
+    <t>tag 2</t>
+  </si>
+  <si>
+    <t>tag 3</t>
+  </si>
+  <si>
+    <t>tag 4</t>
   </si>
 </sst>
 </file>
@@ -826,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1383,4 +2024,1016 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F11E17-5D7E-4788-9486-C9C40FEFD5A6}">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J1" t="s">
+        <v>366</v>
+      </c>
+      <c r="K1" t="s">
+        <v>367</v>
+      </c>
+      <c r="L1" t="s">
+        <v>368</v>
+      </c>
+      <c r="M1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E2" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" t="s">
+        <v>352</v>
+      </c>
+      <c r="K2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" t="s">
+        <v>352</v>
+      </c>
+      <c r="K3" t="s">
+        <v>353</v>
+      </c>
+      <c r="L3" t="s">
+        <v>354</v>
+      </c>
+      <c r="M3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
+        <v>283</v>
+      </c>
+      <c r="H4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" t="s">
+        <v>160</v>
+      </c>
+      <c r="J4" t="s">
+        <v>352</v>
+      </c>
+      <c r="K4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" t="s">
+        <v>260</v>
+      </c>
+      <c r="H5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F7" t="s">
+        <v>286</v>
+      </c>
+      <c r="H7" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7" t="s">
+        <v>355</v>
+      </c>
+      <c r="K7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" t="s">
+        <v>263</v>
+      </c>
+      <c r="H8" t="s">
+        <v>165</v>
+      </c>
+      <c r="J8" t="s">
+        <v>360</v>
+      </c>
+      <c r="K8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J9" t="s">
+        <v>357</v>
+      </c>
+      <c r="K9" t="s">
+        <v>362</v>
+      </c>
+      <c r="L9" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J10" t="s">
+        <v>354</v>
+      </c>
+      <c r="K10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" t="s">
+        <v>267</v>
+      </c>
+      <c r="D12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E12" t="s">
+        <v>289</v>
+      </c>
+      <c r="F12" t="s">
+        <v>288</v>
+      </c>
+      <c r="H12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J12" t="s">
+        <v>362</v>
+      </c>
+      <c r="K12" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" t="s">
+        <v>290</v>
+      </c>
+      <c r="H13" t="s">
+        <v>171</v>
+      </c>
+      <c r="J13" t="s">
+        <v>352</v>
+      </c>
+      <c r="K13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D14" t="s">
+        <v>291</v>
+      </c>
+      <c r="H14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" t="s">
+        <v>361</v>
+      </c>
+      <c r="K14" t="s">
+        <v>362</v>
+      </c>
+      <c r="L14" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" t="s">
+        <v>270</v>
+      </c>
+      <c r="H15" t="s">
+        <v>174</v>
+      </c>
+      <c r="J15" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" t="s">
+        <v>292</v>
+      </c>
+      <c r="H16" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" t="s">
+        <v>272</v>
+      </c>
+      <c r="H17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" t="s">
+        <v>273</v>
+      </c>
+      <c r="H18" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" t="s">
+        <v>293</v>
+      </c>
+      <c r="H19" t="s">
+        <v>179</v>
+      </c>
+      <c r="I19" t="s">
+        <v>178</v>
+      </c>
+      <c r="J19" t="s">
+        <v>357</v>
+      </c>
+      <c r="K19" t="s">
+        <v>362</v>
+      </c>
+      <c r="L19" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C20" t="s">
+        <v>275</v>
+      </c>
+      <c r="H20" t="s">
+        <v>180</v>
+      </c>
+      <c r="J20" t="s">
+        <v>359</v>
+      </c>
+      <c r="K20" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" t="s">
+        <v>276</v>
+      </c>
+      <c r="H21" t="s">
+        <v>181</v>
+      </c>
+      <c r="J21" t="s">
+        <v>353</v>
+      </c>
+      <c r="K21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22" t="s">
+        <v>277</v>
+      </c>
+      <c r="H22" t="s">
+        <v>182</v>
+      </c>
+      <c r="J22" t="s">
+        <v>353</v>
+      </c>
+      <c r="K22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>255</v>
+      </c>
+      <c r="B23" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" t="s">
+        <v>278</v>
+      </c>
+      <c r="H23" t="s">
+        <v>183</v>
+      </c>
+      <c r="J23" t="s">
+        <v>353</v>
+      </c>
+      <c r="K23" t="s">
+        <v>354</v>
+      </c>
+      <c r="L23" t="s">
+        <v>352</v>
+      </c>
+      <c r="M23" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>256</v>
+      </c>
+      <c r="B24" t="s">
+        <v>235</v>
+      </c>
+      <c r="C24" t="s">
+        <v>279</v>
+      </c>
+      <c r="H24" t="s">
+        <v>184</v>
+      </c>
+      <c r="J24" t="s">
+        <v>356</v>
+      </c>
+      <c r="K24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C26" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43AC12E-D22E-4F80-A089-B78B3BB1FB2D}">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J1" t="s">
+        <v>366</v>
+      </c>
+      <c r="K1" t="s">
+        <v>367</v>
+      </c>
+      <c r="L1" t="s">
+        <v>368</v>
+      </c>
+      <c r="M1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
+        <v>327</v>
+      </c>
+      <c r="H2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" t="s">
+        <v>329</v>
+      </c>
+      <c r="H4" t="s">
+        <v>187</v>
+      </c>
+      <c r="J4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" t="s">
+        <v>329</v>
+      </c>
+      <c r="H5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" t="s">
+        <v>330</v>
+      </c>
+      <c r="H6" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" t="s">
+        <v>330</v>
+      </c>
+      <c r="H7" t="s">
+        <v>190</v>
+      </c>
+      <c r="J7" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>331</v>
+      </c>
+      <c r="H8" t="s">
+        <v>191</v>
+      </c>
+      <c r="J8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" t="s">
+        <v>333</v>
+      </c>
+      <c r="H9" t="s">
+        <v>192</v>
+      </c>
+      <c r="J9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>348</v>
+      </c>
+      <c r="B10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" t="s">
+        <v>335</v>
+      </c>
+      <c r="H10" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>349</v>
+      </c>
+      <c r="B11" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" t="s">
+        <v>334</v>
+      </c>
+      <c r="H11" t="s">
+        <v>194</v>
+      </c>
+      <c r="J11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>350</v>
+      </c>
+      <c r="B12" t="s">
+        <v>304</v>
+      </c>
+      <c r="C12" t="s">
+        <v>336</v>
+      </c>
+      <c r="H12" t="s">
+        <v>195</v>
+      </c>
+      <c r="J12" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B13" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" t="s">
+        <v>331</v>
+      </c>
+      <c r="H13" t="s">
+        <v>196</v>
+      </c>
+      <c r="J13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" t="s">
+        <v>334</v>
+      </c>
+      <c r="H14" t="s">
+        <v>197</v>
+      </c>
+      <c r="J14" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B15" t="s">
+        <v>307</v>
+      </c>
+      <c r="C15" t="s">
+        <v>332</v>
+      </c>
+      <c r="H15" t="s">
+        <v>198</v>
+      </c>
+      <c r="J15" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>344</v>
+      </c>
+      <c r="B16" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" t="s">
+        <v>332</v>
+      </c>
+      <c r="H16" t="s">
+        <v>199</v>
+      </c>
+      <c r="J16" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" t="s">
+        <v>309</v>
+      </c>
+      <c r="C17" t="s">
+        <v>336</v>
+      </c>
+      <c r="H17" t="s">
+        <v>200</v>
+      </c>
+      <c r="J17" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>317</v>
+      </c>
+      <c r="B18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C18" t="s">
+        <v>326</v>
+      </c>
+      <c r="H18" t="s">
+        <v>201</v>
+      </c>
+      <c r="J18" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" t="s">
+        <v>325</v>
+      </c>
+      <c r="H19" t="s">
+        <v>202</v>
+      </c>
+      <c r="J19" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>319</v>
+      </c>
+      <c r="B20" t="s">
+        <v>312</v>
+      </c>
+      <c r="C20" t="s">
+        <v>324</v>
+      </c>
+      <c r="H20" t="s">
+        <v>203</v>
+      </c>
+      <c r="J20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>320</v>
+      </c>
+      <c r="B21" t="s">
+        <v>313</v>
+      </c>
+      <c r="C21" t="s">
+        <v>323</v>
+      </c>
+      <c r="H21" t="s">
+        <v>204</v>
+      </c>
+      <c r="J21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>321</v>
+      </c>
+      <c r="B22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" t="s">
+        <v>322</v>
+      </c>
+      <c r="H22" t="s">
+        <v>205</v>
+      </c>
+      <c r="J22" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add urls for the recently added ones; script to fetch official site url from google; codeigniter icon; add ts
</commit_message>
<xml_diff>
--- a/scripts/source.xlsx
+++ b/scripts/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\tomchen\GETICON\geticon\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56F7B92-862A-4901-A8B1-3D35C97DBF6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4016038-310A-463D-B962-9B6670B2ABF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="572">
   <si>
     <t>adobe-acrobat.svg</t>
   </si>
@@ -1630,6 +1630,120 @@
   </si>
   <si>
     <t>streaming</t>
+  </si>
+  <si>
+    <t>https://1password.com/</t>
+  </si>
+  <si>
+    <t>https://www.7-zip.org/</t>
+  </si>
+  <si>
+    <t>https://intl.alipay.com/</t>
+  </si>
+  <si>
+    <t>https://www.openoffice.org/</t>
+  </si>
+  <si>
+    <t>https://bitwarden.com/</t>
+  </si>
+  <si>
+    <t>https://www.daemon-tools.cc/</t>
+  </si>
+  <si>
+    <t>https://www.dashlane.com/</t>
+  </si>
+  <si>
+    <t>https://dev.to/</t>
+  </si>
+  <si>
+    <t>https://evernote.com/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/messenger/</t>
+  </si>
+  <si>
+    <t>https://filezilla-project.org/</t>
+  </si>
+  <si>
+    <t>https://gcc.gnu.org/</t>
+  </si>
+  <si>
+    <t>https://www.gimp.org/</t>
+  </si>
+  <si>
+    <t>https://www.gnome.org/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/earth/</t>
+  </si>
+  <si>
+    <t>https://guix.gnu.org/</t>
+  </si>
+  <si>
+    <t>https://www.kali.org/</t>
+  </si>
+  <si>
+    <t>https://keybase.io/</t>
+  </si>
+  <si>
+    <t>https://www.kuaishou.com/</t>
+  </si>
+  <si>
+    <t>https://www.lastpass.com/</t>
+  </si>
+  <si>
+    <t>https://www.libreoffice.org/</t>
+  </si>
+  <si>
+    <t>https://line.me/</t>
+  </si>
+  <si>
+    <t>https://mega.io/</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365/excel</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365/onedrive</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365/onenote</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365/powerpoint</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365/sharepoint</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-teams</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365/word</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365/yammer</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/microsoft-365</t>
+  </si>
+  <si>
+    <t>https://qzone.qq.com/</t>
+  </si>
+  <si>
+    <t>https://www.snapchat.com/</t>
+  </si>
+  <si>
+    <t>https://www.thunderbird.net/</t>
+  </si>
+  <si>
+    <t>https://www.viber.com/</t>
+  </si>
+  <si>
+    <t>https://www.zhihu.com/</t>
+  </si>
+  <si>
+    <t>https://zoom.us/</t>
   </si>
 </sst>
 </file>
@@ -3536,18 +3650,21 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3601,6 +3718,9 @@
       <c r="B2" t="s">
         <v>422</v>
       </c>
+      <c r="C2" t="s">
+        <v>534</v>
+      </c>
       <c r="H2" t="s">
         <v>371</v>
       </c>
@@ -3618,6 +3738,9 @@
       <c r="B3" t="s">
         <v>423</v>
       </c>
+      <c r="C3" t="s">
+        <v>535</v>
+      </c>
       <c r="H3" t="s">
         <v>372</v>
       </c>
@@ -3632,6 +3755,9 @@
       <c r="B4" t="s">
         <v>424</v>
       </c>
+      <c r="C4" t="s">
+        <v>536</v>
+      </c>
       <c r="D4" t="s">
         <v>516</v>
       </c>
@@ -3655,6 +3781,9 @@
       <c r="B5" t="s">
         <v>425</v>
       </c>
+      <c r="C5" t="s">
+        <v>537</v>
+      </c>
       <c r="D5" t="s">
         <v>512</v>
       </c>
@@ -3684,6 +3813,9 @@
       <c r="B6" t="s">
         <v>426</v>
       </c>
+      <c r="C6" t="s">
+        <v>538</v>
+      </c>
       <c r="H6" t="s">
         <v>378</v>
       </c>
@@ -3701,6 +3833,9 @@
       <c r="B7" t="s">
         <v>427</v>
       </c>
+      <c r="C7" t="s">
+        <v>539</v>
+      </c>
       <c r="H7" t="s">
         <v>379</v>
       </c>
@@ -3712,6 +3847,9 @@
       <c r="B8" t="s">
         <v>428</v>
       </c>
+      <c r="C8" t="s">
+        <v>540</v>
+      </c>
       <c r="H8" t="s">
         <v>381</v>
       </c>
@@ -3729,6 +3867,9 @@
       <c r="B9" t="s">
         <v>429</v>
       </c>
+      <c r="C9" t="s">
+        <v>541</v>
+      </c>
       <c r="D9" t="s">
         <v>510</v>
       </c>
@@ -3749,6 +3890,9 @@
       <c r="B10" t="s">
         <v>430</v>
       </c>
+      <c r="C10" t="s">
+        <v>542</v>
+      </c>
       <c r="H10" t="s">
         <v>383</v>
       </c>
@@ -3763,6 +3907,9 @@
       <c r="B11" t="s">
         <v>431</v>
       </c>
+      <c r="C11" t="s">
+        <v>543</v>
+      </c>
       <c r="D11" t="s">
         <v>509</v>
       </c>
@@ -3780,6 +3927,9 @@
       <c r="B12" t="s">
         <v>432</v>
       </c>
+      <c r="C12" t="s">
+        <v>544</v>
+      </c>
       <c r="H12" t="s">
         <v>386</v>
       </c>
@@ -3791,6 +3941,9 @@
       <c r="B13" t="s">
         <v>433</v>
       </c>
+      <c r="C13" t="s">
+        <v>545</v>
+      </c>
       <c r="H13" t="s">
         <v>387</v>
       </c>
@@ -3802,6 +3955,9 @@
       <c r="B14" t="s">
         <v>434</v>
       </c>
+      <c r="C14" t="s">
+        <v>546</v>
+      </c>
       <c r="H14" t="s">
         <v>388</v>
       </c>
@@ -3816,6 +3972,9 @@
       <c r="B15" t="s">
         <v>435</v>
       </c>
+      <c r="C15" t="s">
+        <v>547</v>
+      </c>
       <c r="H15" t="s">
         <v>389</v>
       </c>
@@ -3827,6 +3986,9 @@
       <c r="B16" t="s">
         <v>436</v>
       </c>
+      <c r="C16" t="s">
+        <v>548</v>
+      </c>
       <c r="H16" t="s">
         <v>390</v>
       </c>
@@ -3841,6 +4003,9 @@
       <c r="B17" t="s">
         <v>437</v>
       </c>
+      <c r="C17" t="s">
+        <v>549</v>
+      </c>
       <c r="D17" t="s">
         <v>508</v>
       </c>
@@ -3858,6 +4023,9 @@
       <c r="B18" t="s">
         <v>438</v>
       </c>
+      <c r="C18" t="s">
+        <v>550</v>
+      </c>
       <c r="D18" t="s">
         <v>507</v>
       </c>
@@ -3878,6 +4046,9 @@
       <c r="B19" t="s">
         <v>439</v>
       </c>
+      <c r="C19" t="s">
+        <v>551</v>
+      </c>
       <c r="H19" t="s">
         <v>394</v>
       </c>
@@ -3892,6 +4063,9 @@
       <c r="B20" t="s">
         <v>440</v>
       </c>
+      <c r="C20" t="s">
+        <v>552</v>
+      </c>
       <c r="D20" t="s">
         <v>506</v>
       </c>
@@ -3918,6 +4092,9 @@
       <c r="B21" t="s">
         <v>441</v>
       </c>
+      <c r="C21" t="s">
+        <v>553</v>
+      </c>
       <c r="H21" t="s">
         <v>397</v>
       </c>
@@ -3935,6 +4112,9 @@
       <c r="B22" t="s">
         <v>442</v>
       </c>
+      <c r="C22" t="s">
+        <v>554</v>
+      </c>
       <c r="H22" t="s">
         <v>399</v>
       </c>
@@ -3952,6 +4132,9 @@
       <c r="B23" t="s">
         <v>443</v>
       </c>
+      <c r="C23" t="s">
+        <v>555</v>
+      </c>
       <c r="H23" t="s">
         <v>401</v>
       </c>
@@ -3966,6 +4149,9 @@
       <c r="B24" t="s">
         <v>444</v>
       </c>
+      <c r="C24" t="s">
+        <v>556</v>
+      </c>
       <c r="H24" t="s">
         <v>403</v>
       </c>
@@ -3983,6 +4169,9 @@
       <c r="B25" t="s">
         <v>445</v>
       </c>
+      <c r="C25" t="s">
+        <v>557</v>
+      </c>
       <c r="D25" t="s">
         <v>498</v>
       </c>
@@ -4006,6 +4195,9 @@
       <c r="B26" t="s">
         <v>446</v>
       </c>
+      <c r="C26" t="s">
+        <v>558</v>
+      </c>
       <c r="D26" t="s">
         <v>499</v>
       </c>
@@ -4029,6 +4221,9 @@
       <c r="B27" t="s">
         <v>447</v>
       </c>
+      <c r="C27" t="s">
+        <v>559</v>
+      </c>
       <c r="D27" t="s">
         <v>500</v>
       </c>
@@ -4052,6 +4247,9 @@
       <c r="B28" t="s">
         <v>448</v>
       </c>
+      <c r="C28" t="s">
+        <v>560</v>
+      </c>
       <c r="D28" t="s">
         <v>501</v>
       </c>
@@ -4075,6 +4273,9 @@
       <c r="B29" t="s">
         <v>449</v>
       </c>
+      <c r="C29" t="s">
+        <v>561</v>
+      </c>
       <c r="D29" t="s">
         <v>502</v>
       </c>
@@ -4098,6 +4299,9 @@
       <c r="B30" t="s">
         <v>450</v>
       </c>
+      <c r="C30" t="s">
+        <v>562</v>
+      </c>
       <c r="D30" t="s">
         <v>503</v>
       </c>
@@ -4127,6 +4331,9 @@
       <c r="B31" t="s">
         <v>451</v>
       </c>
+      <c r="C31" t="s">
+        <v>563</v>
+      </c>
       <c r="D31" t="s">
         <v>504</v>
       </c>
@@ -4150,6 +4357,9 @@
       <c r="B32" t="s">
         <v>421</v>
       </c>
+      <c r="C32" t="s">
+        <v>564</v>
+      </c>
       <c r="D32" t="s">
         <v>517</v>
       </c>
@@ -4173,6 +4383,9 @@
       <c r="B33" t="s">
         <v>452</v>
       </c>
+      <c r="C33" t="s">
+        <v>565</v>
+      </c>
       <c r="H33" t="s">
         <v>412</v>
       </c>
@@ -4193,6 +4406,9 @@
       <c r="B34" t="s">
         <v>453</v>
       </c>
+      <c r="C34" t="s">
+        <v>566</v>
+      </c>
       <c r="D34" t="s">
         <v>496</v>
       </c>
@@ -4213,6 +4429,9 @@
       <c r="B35" t="s">
         <v>454</v>
       </c>
+      <c r="C35" t="s">
+        <v>567</v>
+      </c>
       <c r="H35" t="s">
         <v>414</v>
       </c>
@@ -4227,6 +4446,9 @@
       <c r="B36" t="s">
         <v>455</v>
       </c>
+      <c r="C36" t="s">
+        <v>568</v>
+      </c>
       <c r="D36" t="s">
         <v>495</v>
       </c>
@@ -4244,6 +4466,9 @@
       <c r="B37" t="s">
         <v>456</v>
       </c>
+      <c r="C37" t="s">
+        <v>569</v>
+      </c>
       <c r="D37" t="s">
         <v>493</v>
       </c>
@@ -4264,6 +4489,9 @@
       <c r="B38" t="s">
         <v>457</v>
       </c>
+      <c r="C38" t="s">
+        <v>570</v>
+      </c>
       <c r="D38" t="s">
         <v>497</v>
       </c>
@@ -4286,6 +4514,9 @@
       </c>
       <c r="B39" t="s">
         <v>458</v>
+      </c>
+      <c r="C39" t="s">
+        <v>571</v>
       </c>
       <c r="H39" t="s">
         <v>419</v>

</xml_diff>